<commit_message>
Integrate and expand EDA for UPI analysis
This commit integrates several new Exploratory Data Analysis (EDA) tasks into the existing UPI analysis project.

The `analysis.py` script has been updated to include:
- Yearly and Monthly Trend Analysis with heatmaps for volume and value.
- Outlier Detection for month-over-month growth rates using the IQR method, with plots to visualize outliers.
- Bank Integration Analysis plotting the number of banks vs. transaction volume.

Additionally, the script now generates all visualizations required for the main report, and a new detailed EDA section has been appended to `report.md`.

A `requirements.txt` file has been added to ensure reproducibility of the environment.
</commit_message>
<xml_diff>
--- a/upi_data_cleaned.xlsx
+++ b/upi_data_cleaned.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,36 @@
           <t>Value (in Cr.)</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Volume (in Bn)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Value (in Trn)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Month_Name</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Volume Growth Rate (%)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Value Growth Rate (%)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -474,6 +504,22 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -488,6 +534,22 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -502,6 +564,22 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -516,6 +594,30 @@
       <c r="D5" t="n">
         <v>0.38</v>
       </c>
+      <c r="E5" t="n">
+        <v>8.999999999999999e-05</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.8e-06</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -530,6 +632,26 @@
       <c r="D6" t="n">
         <v>3.09</v>
       </c>
+      <c r="E6" t="n">
+        <v>8.999999999999999e-05</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.09e-05</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>713.1578947368421</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -544,6 +666,26 @@
       <c r="D7" t="n">
         <v>32.64</v>
       </c>
+      <c r="E7" t="n">
+        <v>8.999999999999999e-05</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0003264</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>956.3106796116506</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -558,6 +700,26 @@
       <c r="D8" t="n">
         <v>48.57</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0004857</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>11.11111111111112</v>
+      </c>
+      <c r="J8" t="n">
+        <v>48.80514705882353</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -572,6 +734,26 @@
       <c r="D9" t="n">
         <v>100.46</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.00029</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0010046</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>190</v>
+      </c>
+      <c r="J9" t="n">
+        <v>106.8354951616224</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -586,6 +768,26 @@
       <c r="D10" t="n">
         <v>707.9299999999999</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.00199</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.007079299999999999</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>586.2068965517241</v>
+      </c>
+      <c r="J10" t="n">
+        <v>604.6884332072466</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -600,6 +802,26 @@
       <c r="D11" t="n">
         <v>1696.22</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.00446</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0169622</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>124.1206030150753</v>
+      </c>
+      <c r="J11" t="n">
+        <v>139.6027855861456</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -614,6 +836,26 @@
       <c r="D12" t="n">
         <v>1937.71</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.00438</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0193771</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>-1.793721973094153</v>
+      </c>
+      <c r="J12" t="n">
+        <v>14.23695039558548</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -628,6 +870,26 @@
       <c r="D13" t="n">
         <v>2425.14</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.00637</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0242514</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>45.43378995433789</v>
+      </c>
+      <c r="J13" t="n">
+        <v>25.15495094725215</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -642,6 +904,26 @@
       <c r="D14" t="n">
         <v>2271.24</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.0072</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0227124</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>13.02982731554161</v>
+      </c>
+      <c r="J14" t="n">
+        <v>-6.34602538410155</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -656,6 +938,26 @@
       <c r="D15" t="n">
         <v>2797.07</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.00936</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0279707</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>30</v>
+      </c>
+      <c r="J15" t="n">
+        <v>23.15167045314457</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -670,6 +972,26 @@
       <c r="D16" t="n">
         <v>3098.36</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.01035</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0309836</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>10.57692307692306</v>
+      </c>
+      <c r="J16" t="n">
+        <v>10.77162888308123</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -684,6 +1006,26 @@
       <c r="D17" t="n">
         <v>3411.35</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.01163</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0341135</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>12.36714975845412</v>
+      </c>
+      <c r="J17" t="n">
+        <v>10.10179578873984</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -698,6 +1040,26 @@
       <c r="D18" t="n">
         <v>4156.62</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.0168</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.0415662</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>44.45399828030953</v>
+      </c>
+      <c r="J18" t="n">
+        <v>21.84677620296951</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -712,6 +1074,26 @@
       <c r="D19" t="n">
         <v>5325.81</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.03098</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0532581</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>84.40476190476187</v>
+      </c>
+      <c r="J19" t="n">
+        <v>28.1283831574693</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -726,6 +1108,26 @@
       <c r="D20" t="n">
         <v>7057.78</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.07696</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0705778</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>148.4183344092963</v>
+      </c>
+      <c r="J20" t="n">
+        <v>32.52031146435941</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -740,6 +1142,26 @@
       <c r="D21" t="n">
         <v>9669.33</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.10502</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0966933</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>36.46049896049897</v>
+      </c>
+      <c r="J21" t="n">
+        <v>37.00242852568372</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -754,6 +1176,26 @@
       <c r="D22" t="n">
         <v>13174.24</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.14564</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.1317424</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>38.67834698152733</v>
+      </c>
+      <c r="J22" t="n">
+        <v>36.24770278809392</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -768,6 +1210,26 @@
       <c r="D23" t="n">
         <v>15571.2</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.15183</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.155712</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>4.250205987366118</v>
+      </c>
+      <c r="J23" t="n">
+        <v>18.19429431982416</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -782,6 +1244,26 @@
       <c r="D24" t="n">
         <v>19126.2</v>
       </c>
+      <c r="E24" t="n">
+        <v>0.1714</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.191262</v>
+      </c>
+      <c r="G24" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>12.88941579398008</v>
+      </c>
+      <c r="J24" t="n">
+        <v>22.83061035758323</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -796,6 +1278,26 @@
       <c r="D25" t="n">
         <v>24172.6</v>
       </c>
+      <c r="E25" t="n">
+        <v>0.17805</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.241726</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>3.87981330221705</v>
+      </c>
+      <c r="J25" t="n">
+        <v>26.38474971505054</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -810,6 +1312,26 @@
       <c r="D26" t="n">
         <v>27021.85</v>
       </c>
+      <c r="E26" t="n">
+        <v>0.19008</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.2702185</v>
+      </c>
+      <c r="G26" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>6.75652906486941</v>
+      </c>
+      <c r="J26" t="n">
+        <v>11.78710606223574</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -824,6 +1346,26 @@
       <c r="D27" t="n">
         <v>33288.51</v>
       </c>
+      <c r="E27" t="n">
+        <v>0.18948</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.3328851</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>-0.3156565656565746</v>
+      </c>
+      <c r="J27" t="n">
+        <v>23.19108425218854</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -838,6 +1380,26 @@
       <c r="D28" t="n">
         <v>40834.03</v>
       </c>
+      <c r="E28" t="n">
+        <v>0.24637</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.4083403</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>30.0242769685455</v>
+      </c>
+      <c r="J28" t="n">
+        <v>22.66704036918443</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -852,6 +1414,26 @@
       <c r="D29" t="n">
         <v>51843.14</v>
       </c>
+      <c r="E29" t="n">
+        <v>0.27375</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.5184314</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>11.11336607541502</v>
+      </c>
+      <c r="J29" t="n">
+        <v>26.96062573299769</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -866,6 +1448,26 @@
       <c r="D30" t="n">
         <v>54212.26</v>
       </c>
+      <c r="E30" t="n">
+        <v>0.31202</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.5421226</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>13.97990867579908</v>
+      </c>
+      <c r="J30" t="n">
+        <v>4.569784932008369</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -880,6 +1482,26 @@
       <c r="D31" t="n">
         <v>59835.36</v>
       </c>
+      <c r="E31" t="n">
+        <v>0.40587</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.5983536</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>30.07820011537723</v>
+      </c>
+      <c r="J31" t="n">
+        <v>10.37237702320473</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -894,6 +1516,26 @@
       <c r="D32" t="n">
         <v>74978.27</v>
       </c>
+      <c r="E32" t="n">
+        <v>0.48236</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.7497827</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>18.84593589080248</v>
+      </c>
+      <c r="J32" t="n">
+        <v>25.30762746309205</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -908,6 +1550,26 @@
       <c r="D33" t="n">
         <v>82232.21000000001</v>
       </c>
+      <c r="E33" t="n">
+        <v>0.5249400000000001</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.8223221000000001</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>8.827431793681084</v>
+      </c>
+      <c r="J33" t="n">
+        <v>9.674723089769888</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -922,6 +1584,26 @@
       <c r="D34" t="n">
         <v>102594.82</v>
       </c>
+      <c r="E34" t="n">
+        <v>0.62017</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1.0259482</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>18.14112089000646</v>
+      </c>
+      <c r="J34" t="n">
+        <v>24.76232853282185</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -936,6 +1618,26 @@
       <c r="D35" t="n">
         <v>109932.43</v>
       </c>
+      <c r="E35" t="n">
+        <v>0.67275</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.0993243</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>8.478320460518884</v>
+      </c>
+      <c r="J35" t="n">
+        <v>7.152027753447965</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -950,6 +1652,26 @@
       <c r="D36" t="n">
         <v>106737.12</v>
       </c>
+      <c r="E36" t="n">
+        <v>0.6741900000000001</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1.0673712</v>
+      </c>
+      <c r="G36" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>0.2140468227424863</v>
+      </c>
+      <c r="J36" t="n">
+        <v>-2.906612725653379</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -964,6 +1686,26 @@
       <c r="D37" t="n">
         <v>133460.72</v>
       </c>
+      <c r="E37" t="n">
+        <v>0.7995399999999999</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1.3346072</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>18.59268158827627</v>
+      </c>
+      <c r="J37" t="n">
+        <v>25.03683816838977</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -978,6 +1720,26 @@
       <c r="D38" t="n">
         <v>142034.39</v>
       </c>
+      <c r="E38" t="n">
+        <v>0.78179</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1.4203439</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>-2.220026515246254</v>
+      </c>
+      <c r="J38" t="n">
+        <v>6.424114900623956</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -992,6 +1754,26 @@
       <c r="D39" t="n">
         <v>152449.29</v>
       </c>
+      <c r="E39" t="n">
+        <v>0.73354</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1.5244929</v>
+      </c>
+      <c r="G39" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>-6.17173409739189</v>
+      </c>
+      <c r="J39" t="n">
+        <v>7.33266077321133</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -1006,6 +1788,26 @@
       <c r="D40" t="n">
         <v>146566.35</v>
       </c>
+      <c r="E40" t="n">
+        <v>0.75454</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1.4656635</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>2.862829566213154</v>
+      </c>
+      <c r="J40" t="n">
+        <v>-3.858948769128412</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -1020,6 +1822,26 @@
       <c r="D41" t="n">
         <v>146386.64</v>
       </c>
+      <c r="E41" t="n">
+        <v>0.82229</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1.4638664</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>8.978980570943884</v>
+      </c>
+      <c r="J41" t="n">
+        <v>-0.1226134102404686</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -1034,6 +1856,26 @@
       <c r="D42" t="n">
         <v>154504.89</v>
       </c>
+      <c r="E42" t="n">
+        <v>0.91835</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1.5450489</v>
+      </c>
+      <c r="G42" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>11.68200999647326</v>
+      </c>
+      <c r="J42" t="n">
+        <v>5.545758820613678</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -1048,6 +1890,26 @@
       <c r="D43" t="n">
         <v>161456.56</v>
       </c>
+      <c r="E43" t="n">
+        <v>0.95502</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1.6145656</v>
+      </c>
+      <c r="G43" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>3.993030979474055</v>
+      </c>
+      <c r="J43" t="n">
+        <v>4.499320377497429</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -1062,6 +1924,26 @@
       <c r="D44" t="n">
         <v>191359.94</v>
       </c>
+      <c r="E44" t="n">
+        <v>1.14836</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1.9135994</v>
+      </c>
+      <c r="G44" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>20.24460220728359</v>
+      </c>
+      <c r="J44" t="n">
+        <v>18.52100651717095</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -1076,6 +1958,26 @@
       <c r="D45" t="n">
         <v>189229.09</v>
       </c>
+      <c r="E45" t="n">
+        <v>1.21877</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1.8922909</v>
+      </c>
+      <c r="G45" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>6.131352537531787</v>
+      </c>
+      <c r="J45" t="n">
+        <v>-1.113529822386028</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -1090,6 +1992,26 @@
       <c r="D46" t="n">
         <v>202520.76</v>
       </c>
+      <c r="E46" t="n">
+        <v>1.3084</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2.0252076</v>
+      </c>
+      <c r="G46" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>7.354135727003452</v>
+      </c>
+      <c r="J46" t="n">
+        <v>7.024115583919999</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -1104,6 +2026,26 @@
       <c r="D47" t="n">
         <v>216242.97</v>
       </c>
+      <c r="E47" t="n">
+        <v>1.30502</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2.1624297</v>
+      </c>
+      <c r="G47" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>-0.2583307856924399</v>
+      </c>
+      <c r="J47" t="n">
+        <v>6.775705364724094</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -1118,6 +2060,26 @@
       <c r="D48" t="n">
         <v>222516.95</v>
       </c>
+      <c r="E48" t="n">
+        <v>1.32569</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2.2251695</v>
+      </c>
+      <c r="G48" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>1.583883771896222</v>
+      </c>
+      <c r="J48" t="n">
+        <v>2.901356746996231</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -1131,6 +2093,26 @@
       </c>
       <c r="D49" t="n">
         <v>206462.31</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.24684</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2.0646231</v>
+      </c>
+      <c r="G49" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>-5.947846027351799</v>
+      </c>
+      <c r="J49" t="n">
+        <v>-7.215018900807346</v>
       </c>
     </row>
   </sheetData>
@@ -1144,7 +2126,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1173,6 +2155,36 @@
           <t>Value (in Cr.)</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Volume (in Bn)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Value (in Trn)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Month_Name</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Volume Growth Rate (%)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Value Growth Rate (%)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -1187,6 +2199,26 @@
       <c r="D2" t="n">
         <v>151140.66</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.9995700000000001</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.5114066</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>-19.83173462513232</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-26.79503585908731</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -1201,6 +2233,26 @@
       <c r="D3" t="n">
         <v>218391.6</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.2345</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.183916</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>23.50310633572434</v>
+      </c>
+      <c r="J3" t="n">
+        <v>44.49559767702485</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -1215,6 +2267,26 @@
       <c r="D4" t="n">
         <v>261835</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.33693</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.61835</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>8.29728635074931</v>
+      </c>
+      <c r="J4" t="n">
+        <v>19.8924317601959</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -1229,6 +2301,26 @@
       <c r="D5" t="n">
         <v>290537.86</v>
       </c>
+      <c r="E5" t="n">
+        <v>1.49736</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.9053786</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>11.99988032282915</v>
+      </c>
+      <c r="J5" t="n">
+        <v>10.96219374797105</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -1243,6 +2335,26 @@
       <c r="D6" t="n">
         <v>298307.61</v>
       </c>
+      <c r="E6" t="n">
+        <v>1.61883</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.9830761</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>8.112277608591123</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2.674264207769683</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -1257,6 +2369,26 @@
       <c r="D7" t="n">
         <v>329027.66</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.80014</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.2902766</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>11.20006424392925</v>
+      </c>
+      <c r="J7" t="n">
+        <v>10.2981114025217</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1271,6 +2403,26 @@
       <c r="D8" t="n">
         <v>386106.74</v>
       </c>
+      <c r="E8" t="n">
+        <v>2.07162</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.8610674</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>15.08104925172484</v>
+      </c>
+      <c r="J8" t="n">
+        <v>17.34780595649619</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -1285,6 +2437,26 @@
       <c r="D9" t="n">
         <v>390999.15</v>
       </c>
+      <c r="E9" t="n">
+        <v>2.21023</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3.9099915</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>6.690898910031784</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.267113337622661</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -1299,6 +2471,26 @@
       <c r="D10" t="n">
         <v>416176.21</v>
       </c>
+      <c r="E10" t="n">
+        <v>2.23416</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.1617621</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>1.08269275143309</v>
+      </c>
+      <c r="J10" t="n">
+        <v>6.439159778224579</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -1313,6 +2505,26 @@
       <c r="D11" t="n">
         <v>431181.89</v>
       </c>
+      <c r="E11" t="n">
+        <v>2.30273</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4.3118189</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>3.069162459268826</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3.605607345984541</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1327,6 +2539,26 @@
       <c r="D12" t="n">
         <v>425062.76</v>
       </c>
+      <c r="E12" t="n">
+        <v>2.2929</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4.250627600000001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>-0.4268846108749225</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-1.419152831302817</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -1341,6 +2573,26 @@
       <c r="D13" t="n">
         <v>504886.44</v>
       </c>
+      <c r="E13" t="n">
+        <v>2.73168</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5.0488644</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>19.13646473897683</v>
+      </c>
+      <c r="J13" t="n">
+        <v>18.77926920721071</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -1355,6 +2607,26 @@
       <c r="D14" t="n">
         <v>493663.68</v>
       </c>
+      <c r="E14" t="n">
+        <v>2.64106</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4.9366368</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>-3.317372459438872</v>
+      </c>
+      <c r="J14" t="n">
+        <v>-2.22282856319137</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -1369,6 +2641,26 @@
       <c r="D15" t="n">
         <v>490638.65</v>
       </c>
+      <c r="E15" t="n">
+        <v>2.53957</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4.9063865</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>-3.842775249331698</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-0.6127714317569311</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -1383,6 +2675,26 @@
       <c r="D16" t="n">
         <v>547373.17</v>
       </c>
+      <c r="E16" t="n">
+        <v>2.80751</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5.4737317</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>10.5506050236851</v>
+      </c>
+      <c r="J16" t="n">
+        <v>11.5634021086598</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -1397,6 +2709,26 @@
       <c r="D17" t="n">
         <v>606281.14</v>
       </c>
+      <c r="E17" t="n">
+        <v>3.24782</v>
+      </c>
+      <c r="F17" t="n">
+        <v>6.0628114</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>15.68329231240495</v>
+      </c>
+      <c r="J17" t="n">
+        <v>10.76193961059508</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -1411,6 +2743,26 @@
       <c r="D18" t="n">
         <v>639116.95</v>
       </c>
+      <c r="E18" t="n">
+        <v>3.55555</v>
+      </c>
+      <c r="F18" t="n">
+        <v>6.391169499999999</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>9.47497090355991</v>
+      </c>
+      <c r="J18" t="n">
+        <v>5.415937893103506</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -1425,6 +2777,26 @@
       <c r="D19" t="n">
         <v>654351.8100000001</v>
       </c>
+      <c r="E19" t="n">
+        <v>3.6543</v>
+      </c>
+      <c r="F19" t="n">
+        <v>6.543518100000001</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>2.777348089606391</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2.38373587181504</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -1439,6 +2811,26 @@
       <c r="D20" t="n">
         <v>771444.98</v>
       </c>
+      <c r="E20" t="n">
+        <v>4.218649999999999</v>
+      </c>
+      <c r="F20" t="n">
+        <v>7.7144498</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>15.44345018197737</v>
+      </c>
+      <c r="J20" t="n">
+        <v>17.8945283272006</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -1453,6 +2845,26 @@
       <c r="D21" t="n">
         <v>768436.11</v>
       </c>
+      <c r="E21" t="n">
+        <v>4.18648</v>
+      </c>
+      <c r="F21" t="n">
+        <v>7.6843611</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>-0.7625662237919717</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-0.3900304076124739</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -1467,6 +2879,26 @@
       <c r="D22" t="n">
         <v>826848.22</v>
       </c>
+      <c r="E22" t="n">
+        <v>4.5663</v>
+      </c>
+      <c r="F22" t="n">
+        <v>8.268482199999999</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>9.072538266037355</v>
+      </c>
+      <c r="J22" t="n">
+        <v>7.601427007379957</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -1480,6 +2912,26 @@
       </c>
       <c r="D23" t="n">
         <v>831993.11</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4.61715</v>
+      </c>
+      <c r="F23" t="n">
+        <v>8.3199311</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2022</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>1.113593062216656</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.6222290712556644</v>
       </c>
     </row>
   </sheetData>
@@ -1493,7 +2945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1522,6 +2974,36 @@
           <t>Value (in Cr.)</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Volume (in Bn)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Value (in Trn)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Month_Name</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Volume Growth Rate (%)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Value Growth Rate (%)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -1536,6 +3018,26 @@
       <c r="D2" t="n">
         <v>1072792.68</v>
       </c>
+      <c r="E2" t="n">
+        <v>6.57963</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10.7279268</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>4.631225748998169</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.9220127915196441</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -1550,6 +3052,26 @@
       <c r="D3" t="n">
         <v>1116438.1</v>
       </c>
+      <c r="E3" t="n">
+        <v>6.7808</v>
+      </c>
+      <c r="F3" t="n">
+        <v>11.164381</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2022</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>3.057466757249272</v>
+      </c>
+      <c r="J3" t="n">
+        <v>4.068392785827002</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -1564,6 +3086,26 @@
       <c r="D4" t="n">
         <v>1211582.51</v>
       </c>
+      <c r="E4" t="n">
+        <v>7.30542</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12.1158251</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>7.736845210004706</v>
+      </c>
+      <c r="J4" t="n">
+        <v>8.522139292809872</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -1578,6 +3120,26 @@
       <c r="D5" t="n">
         <v>1190593.39</v>
       </c>
+      <c r="E5" t="n">
+        <v>7.30945</v>
+      </c>
+      <c r="F5" t="n">
+        <v>11.9059339</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0.05516452168390362</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-1.732372316929542</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -1592,6 +3154,26 @@
       <c r="D6" t="n">
         <v>1282055.01</v>
       </c>
+      <c r="E6" t="n">
+        <v>7.82949</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12.8205501</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2022</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>7.114625587424506</v>
+      </c>
+      <c r="J6" t="n">
+        <v>7.682019803587203</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -1606,6 +3188,26 @@
       <c r="D7" t="n">
         <v>1298726.62</v>
       </c>
+      <c r="E7" t="n">
+        <v>8.03689</v>
+      </c>
+      <c r="F7" t="n">
+        <v>12.9872662</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>2.648959255328243</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.300381798749806</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1620,6 +3222,26 @@
       <c r="D8" t="n">
         <v>1235846.62</v>
       </c>
+      <c r="E8" t="n">
+        <v>7.53476</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12.3584662</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>-6.247814764168713</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-4.841665600109124</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -1634,6 +3256,26 @@
       <c r="D9" t="n">
         <v>1410443.01</v>
       </c>
+      <c r="E9" t="n">
+        <v>8.6853</v>
+      </c>
+      <c r="F9" t="n">
+        <v>14.1044301</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>15.26976307141832</v>
+      </c>
+      <c r="J9" t="n">
+        <v>14.12767467859402</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -1648,6 +3290,26 @@
       <c r="D10" t="n">
         <v>1415504.71</v>
       </c>
+      <c r="E10" t="n">
+        <v>8.86326</v>
+      </c>
+      <c r="F10" t="n">
+        <v>14.1550471</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>2.048979309868404</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.3588730607413826</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -1662,6 +3324,26 @@
       <c r="D11" t="n">
         <v>1489145.44</v>
       </c>
+      <c r="E11" t="n">
+        <v>9.415190000000001</v>
+      </c>
+      <c r="F11" t="n">
+        <v>14.8914544</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>6.227166979192766</v>
+      </c>
+      <c r="J11" t="n">
+        <v>5.202436239155994</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1676,6 +3358,26 @@
       <c r="D12" t="n">
         <v>1475464.26</v>
       </c>
+      <c r="E12" t="n">
+        <v>9.33506</v>
+      </c>
+      <c r="F12" t="n">
+        <v>14.7546426</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>-0.8510715131611835</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-0.9187269176340385</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -1690,6 +3392,26 @@
       <c r="D13" t="n">
         <v>1533536.44</v>
       </c>
+      <c r="E13" t="n">
+        <v>9.96461</v>
+      </c>
+      <c r="F13" t="n">
+        <v>15.3353644</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>6.743930944203891</v>
+      </c>
+      <c r="J13" t="n">
+        <v>3.935858127800396</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -1704,6 +3426,26 @@
       <c r="D14" t="n">
         <v>1576536.56</v>
       </c>
+      <c r="E14" t="n">
+        <v>10.58602</v>
+      </c>
+      <c r="F14" t="n">
+        <v>15.7653656</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>6.236169804939684</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2.803984233984047</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -1718,6 +3460,26 @@
       <c r="D15" t="n">
         <v>1579133.18</v>
       </c>
+      <c r="E15" t="n">
+        <v>10.55569</v>
+      </c>
+      <c r="F15" t="n">
+        <v>15.7913318</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>-0.2865099442472374</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.1647040776523445</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -1732,6 +3494,26 @@
       <c r="D16" t="n">
         <v>1715768.34</v>
       </c>
+      <c r="E16" t="n">
+        <v>11.40879</v>
+      </c>
+      <c r="F16" t="n">
+        <v>17.1576834</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>8.081897062153232</v>
+      </c>
+      <c r="J16" t="n">
+        <v>8.652541896434606</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -1746,6 +3528,26 @@
       <c r="D17" t="n">
         <v>1739740.61</v>
       </c>
+      <c r="E17" t="n">
+        <v>11.23529</v>
+      </c>
+      <c r="F17" t="n">
+        <v>17.3974061</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>-1.520757240688986</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1.397174049732164</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -1760,6 +3562,26 @@
       <c r="D18" t="n">
         <v>1822949.42</v>
       </c>
+      <c r="E18" t="n">
+        <v>12.02023</v>
+      </c>
+      <c r="F18" t="n">
+        <v>18.2294942</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>6.986379523804009</v>
+      </c>
+      <c r="J18" t="n">
+        <v>4.782828516028004</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -1774,6 +3596,26 @@
       <c r="D19" t="n">
         <v>1841083.97</v>
       </c>
+      <c r="E19" t="n">
+        <v>12.20302</v>
+      </c>
+      <c r="F19" t="n">
+        <v>18.4108397</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>1.520686376217428</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.9947917260370476</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -1788,6 +3630,26 @@
       <c r="D20" t="n">
         <v>1827869.35</v>
       </c>
+      <c r="E20" t="n">
+        <v>12.10267</v>
+      </c>
+      <c r="F20" t="n">
+        <v>18.2786935</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>-0.8223374213924162</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-0.7177630252247602</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -1802,6 +3664,26 @@
       <c r="D21" t="n">
         <v>1978353.23</v>
       </c>
+      <c r="E21" t="n">
+        <v>13.44</v>
+      </c>
+      <c r="F21" t="n">
+        <v>19.7835323</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>11.04987577121412</v>
+      </c>
+      <c r="J21" t="n">
+        <v>8.23274814471835</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -1816,6 +3698,26 @@
       <c r="D22" t="n">
         <v>1964464.52</v>
       </c>
+      <c r="E22" t="n">
+        <v>13.30399</v>
+      </c>
+      <c r="F22" t="n">
+        <v>19.6446452</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>-1.011979166666654</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-0.7020338829987538</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -1830,6 +3732,26 @@
       <c r="D23" t="n">
         <v>2044937.05</v>
       </c>
+      <c r="E23" t="n">
+        <v>14.03584</v>
+      </c>
+      <c r="F23" t="n">
+        <v>20.4493705</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>5.500981284562001</v>
+      </c>
+      <c r="J23" t="n">
+        <v>4.096410455913957</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -1844,6 +3766,26 @@
       <c r="D24" t="n">
         <v>2007081.2</v>
       </c>
+      <c r="E24" t="n">
+        <v>13.88514</v>
+      </c>
+      <c r="F24" t="n">
+        <v>20.070812</v>
+      </c>
+      <c r="G24" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>-1.073679950754647</v>
+      </c>
+      <c r="J24" t="n">
+        <v>-1.851198793625464</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -1858,6 +3800,26 @@
       <c r="D25" t="n">
         <v>2064292.41</v>
       </c>
+      <c r="E25" t="n">
+        <v>14.43555</v>
+      </c>
+      <c r="F25" t="n">
+        <v>20.6429241</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>3.964021968809828</v>
+      </c>
+      <c r="J25" t="n">
+        <v>2.85046813252996</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -1872,6 +3834,26 @@
       <c r="D26" t="n">
         <v>2060735.57</v>
       </c>
+      <c r="E26" t="n">
+        <v>14.96305</v>
+      </c>
+      <c r="F26" t="n">
+        <v>20.6073557</v>
+      </c>
+      <c r="G26" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>3.654173204346223</v>
+      </c>
+      <c r="J26" t="n">
+        <v>-0.1723031089379434</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -1886,6 +3868,26 @@
       <c r="D27" t="n">
         <v>2063994.71</v>
       </c>
+      <c r="E27" t="n">
+        <v>15.04175</v>
+      </c>
+      <c r="F27" t="n">
+        <v>20.6399471</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>0.5259622871005565</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.1581542070436592</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -1900,6 +3902,26 @@
       <c r="D28" t="n">
         <v>2349821.46</v>
       </c>
+      <c r="E28" t="n">
+        <v>16.58497</v>
+      </c>
+      <c r="F28" t="n">
+        <v>23.4982146</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>10.25957750926589</v>
+      </c>
+      <c r="J28" t="n">
+        <v>13.84823074473869</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -1914,6 +3936,26 @@
       <c r="D29" t="n">
         <v>2155187.4</v>
       </c>
+      <c r="E29" t="n">
+        <v>15.48202</v>
+      </c>
+      <c r="F29" t="n">
+        <v>21.551874</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>-6.650298432858193</v>
+      </c>
+      <c r="J29" t="n">
+        <v>-8.28292971671134</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -1928,6 +3970,26 @@
       <c r="D30" t="n">
         <v>2324699.91</v>
       </c>
+      <c r="E30" t="n">
+        <v>16.73001</v>
+      </c>
+      <c r="F30" t="n">
+        <v>23.2469991</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>8.060899029971536</v>
+      </c>
+      <c r="J30" t="n">
+        <v>7.865325771670717</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -1942,6 +4004,26 @@
       <c r="D31" t="n">
         <v>2348037.12</v>
       </c>
+      <c r="E31" t="n">
+        <v>16.996</v>
+      </c>
+      <c r="F31" t="n">
+        <v>23.4803712</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>1.589897435805465</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1.003880539574675</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -1956,6 +4038,26 @@
       <c r="D32" t="n">
         <v>2196481.69</v>
       </c>
+      <c r="E32" t="n">
+        <v>16.10619</v>
+      </c>
+      <c r="F32" t="n">
+        <v>21.9648169</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>-5.235408331372071</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-6.45455852077842</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -1970,6 +4072,26 @@
       <c r="D33" t="n">
         <v>2477221.61</v>
       </c>
+      <c r="E33" t="n">
+        <v>18.30151</v>
+      </c>
+      <c r="F33" t="n">
+        <v>24.7722161</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>13.63028748574302</v>
+      </c>
+      <c r="J33" t="n">
+        <v>12.78134578941106</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -1984,6 +4106,26 @@
       <c r="D34" t="n">
         <v>2394925.87</v>
       </c>
+      <c r="E34" t="n">
+        <v>17.89342</v>
+      </c>
+      <c r="F34" t="n">
+        <v>23.9492587</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>-2.229816009717223</v>
+      </c>
+      <c r="J34" t="n">
+        <v>-3.322098421384256</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -1998,6 +4140,26 @@
       <c r="D35" t="n">
         <v>2514297.01</v>
       </c>
+      <c r="E35" t="n">
+        <v>18.67746</v>
+      </c>
+      <c r="F35" t="n">
+        <v>25.1429701</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>4.381722443222147</v>
+      </c>
+      <c r="J35" t="n">
+        <v>4.984335485924651</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -2012,6 +4174,26 @@
       <c r="D36" t="n">
         <v>2403930.69</v>
       </c>
+      <c r="E36" t="n">
+        <v>18.39501</v>
+      </c>
+      <c r="F36" t="n">
+        <v>24.0393069</v>
+      </c>
+      <c r="G36" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>-1.512250595102338</v>
+      </c>
+      <c r="J36" t="n">
+        <v>-4.389549824903138</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -2025,6 +4207,26 @@
       </c>
       <c r="D37" t="n">
         <v>2508498.09</v>
+      </c>
+      <c r="E37" t="n">
+        <v>19.46795</v>
+      </c>
+      <c r="F37" t="n">
+        <v>25.0849809</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>5.832777476065543</v>
+      </c>
+      <c r="J37" t="n">
+        <v>4.349850868620497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>